<commit_message>
inserted all module to top level design
</commit_message>
<xml_diff>
--- a/HSID_RCB_RevB.xlsx
+++ b/HSID_RCB_RevB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\FPGA\git\RCB_Rev_B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC3EE11-768B-4EA8-BA42-920BD541DA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4911CED9-EBDF-46FD-8C8E-0A1D48E53CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9B9F24D7-41B0-450D-BA52-4B08206AAC62}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9B9F24D7-41B0-450D-BA52-4B08206AAC62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="238">
   <si>
     <t>reg</t>
   </si>
@@ -71,15 +71,6 @@
     <t>BIT_SSR_SW</t>
   </si>
   <si>
-    <t>ESTOP_DELAY</t>
-  </si>
-  <si>
-    <t>ESTOP_OPEN_REQUEST</t>
-  </si>
-  <si>
-    <t>ESTOP_STATUS</t>
-  </si>
-  <si>
     <t>ESTOP_STATUS_FAIL</t>
   </si>
   <si>
@@ -89,9 +80,6 @@
     <t>FPGA_DIAG_ACT</t>
   </si>
   <si>
-    <t>FPGA_ESTOP_REQ</t>
-  </si>
-  <si>
     <t>FPGA_FAULT</t>
   </si>
   <si>
@@ -335,9 +323,6 @@
     <t>0x0002</t>
   </si>
   <si>
-    <t>SSRs</t>
-  </si>
-  <si>
     <t>bit0</t>
   </si>
   <si>
@@ -437,12 +422,6 @@
     <t>0x0003</t>
   </si>
   <si>
-    <t>Diagnostic packed counter</t>
-  </si>
-  <si>
-    <t>Diagnostic error counter</t>
-  </si>
-  <si>
     <t>0x0004</t>
   </si>
   <si>
@@ -629,12 +608,6 @@
     <t>0x000F</t>
   </si>
   <si>
-    <t>FLA R</t>
-  </si>
-  <si>
-    <t>FLA L</t>
-  </si>
-  <si>
     <t>00-L_TOOL_EX ,01-L LED Strip ,10-R Tool Ex, 11-R LED Stirp,100-WS LED Strip,101-Robot ESTOP LED</t>
   </si>
   <si>
@@ -704,12 +677,6 @@
     <t>Mic.C.B</t>
   </si>
   <si>
-    <t>D.C</t>
-  </si>
-  <si>
-    <t>Sync counter</t>
-  </si>
-  <si>
     <t>ADC Voltage 0</t>
   </si>
   <si>
@@ -747,6 +714,42 @@
   </si>
   <si>
     <t>FPGA Spare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSRs Left </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSRs Right </t>
+  </si>
+  <si>
+    <t>CS_ERROR</t>
+  </si>
+  <si>
+    <t>FLA PS</t>
+  </si>
+  <si>
+    <t>Fault Registers</t>
+  </si>
+  <si>
+    <t>0x001C</t>
+  </si>
+  <si>
+    <t>0x001D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sync Timer </t>
+  </si>
+  <si>
+    <t>counts time from Mic.C.B rising in uSec</t>
+  </si>
+  <si>
+    <t>time from Mic.C.B rising in uSec</t>
+  </si>
+  <si>
+    <t>Left Diagnostic counter</t>
+  </si>
+  <si>
+    <t>Right Diagnostic counter</t>
   </si>
 </sst>
 </file>
@@ -800,7 +803,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -814,6 +817,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1148,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B1DA1C-2C46-416D-A8B7-01E6D657AEE6}">
-  <dimension ref="A1:AJ44"/>
+  <dimension ref="A1:AJ31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,8 +1165,7 @@
     <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
     <col min="5" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1175,120 +1178,120 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" t="s">
         <v>100</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>101</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>102</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>103</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>104</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>105</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" t="s">
         <v>106</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
         <v>107</v>
       </c>
-      <c r="M1" t="s">
+      <c r="R1" t="s">
         <v>108</v>
       </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
         <v>109</v>
       </c>
-      <c r="O1" t="s">
+      <c r="T1" t="s">
         <v>110</v>
       </c>
-      <c r="P1" t="s">
+      <c r="U1" t="s">
         <v>111</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="V1" t="s">
         <v>112</v>
       </c>
-      <c r="R1" t="s">
+      <c r="W1" t="s">
         <v>113</v>
       </c>
-      <c r="S1" t="s">
+      <c r="X1" t="s">
         <v>114</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Y1" t="s">
         <v>115</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Z1" t="s">
         <v>116</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AA1" t="s">
         <v>117</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AB1" t="s">
         <v>118</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AC1" t="s">
         <v>119</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AD1" t="s">
         <v>120</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AE1" t="s">
         <v>121</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AF1" t="s">
         <v>122</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AG1" t="s">
         <v>123</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AH1" t="s">
         <v>124</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AI1" t="s">
         <v>125</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AJ1" t="s">
         <v>126</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>129</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>130</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -1298,7 +1301,7 @@
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
@@ -1308,7 +1311,7 @@
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
       <c r="U2" s="6" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
@@ -1328,18 +1331,18 @@
     </row>
     <row r="3" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="E3" s="6"/>
+        <v>91</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="6" t="s">
+        <v>181</v>
+      </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -1348,7 +1351,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
@@ -1358,7 +1361,7 @@
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
       <c r="U3" s="6" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="V3" s="6"/>
       <c r="W3" s="6"/>
@@ -1368,7 +1371,7 @@
       <c r="AA3" s="6"/>
       <c r="AB3" s="6"/>
       <c r="AC3" s="6" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="AD3" s="6"/>
       <c r="AE3" s="6"/>
@@ -1380,141 +1383,141 @@
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B5" t="s">
-        <v>190</v>
-      </c>
-      <c r="C5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="C6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="J6" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="F6" t="s">
+      <c r="M6" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="G6" t="s">
+      <c r="N6" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="H6" t="s">
+      <c r="O6" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="I6" t="s">
+      <c r="P6" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="J6" t="s">
+    </row>
+    <row r="7" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="K6" t="s">
+      <c r="F7" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="L6" t="s">
+      <c r="G7" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="M6" t="s">
+      <c r="H7" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="N6" t="s">
+      <c r="I7" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="O6" t="s">
+      <c r="J7" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="P6" t="s">
+      <c r="K7" s="5" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B7" t="s">
-        <v>141</v>
-      </c>
-      <c r="C7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="L7" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="F7" t="s">
+      <c r="M7" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="G7" t="s">
+      <c r="N7" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="H7" t="s">
+      <c r="O7" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="I7" t="s">
+      <c r="P7" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="J7" t="s">
-        <v>160</v>
-      </c>
-      <c r="K7" t="s">
-        <v>161</v>
-      </c>
-      <c r="L7" t="s">
-        <v>162</v>
-      </c>
-      <c r="M7" t="s">
-        <v>163</v>
-      </c>
-      <c r="N7" t="s">
-        <v>164</v>
-      </c>
-      <c r="O7" t="s">
-        <v>165</v>
-      </c>
-      <c r="P7" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>236</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -1531,7 +1534,9 @@
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
+      <c r="U8" s="3" t="s">
+        <v>173</v>
+      </c>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
@@ -1550,16 +1555,16 @@
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>237</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -1576,7 +1581,9 @@
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
+      <c r="U9" s="3" t="s">
+        <v>173</v>
+      </c>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
@@ -1595,184 +1602,185 @@
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B10" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" t="s">
         <v>59</v>
-      </c>
-      <c r="G10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H10" t="s">
-        <v>64</v>
-      </c>
-      <c r="I10" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B11" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" t="s">
         <v>34</v>
       </c>
-      <c r="G11" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>191</v>
-      </c>
-      <c r="B12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12" t="s">
+    </row>
+    <row r="12" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I12" t="s">
+    </row>
+    <row r="13" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J12" t="s">
+      <c r="F13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K12" t="s">
+      <c r="G13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L12" t="s">
+      <c r="H13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M12" t="s">
+      <c r="I13" s="5" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B14" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C14" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" t="s">
         <v>40</v>
       </c>
-      <c r="F14" t="s">
+      <c r="J14" t="s">
         <v>41</v>
       </c>
-      <c r="G14" t="s">
+      <c r="K14" t="s">
         <v>42</v>
       </c>
-      <c r="H14" t="s">
+      <c r="L14" t="s">
         <v>43</v>
-      </c>
-      <c r="I14" t="s">
-        <v>44</v>
-      </c>
-      <c r="J14" t="s">
-        <v>45</v>
-      </c>
-      <c r="K14" t="s">
-        <v>46</v>
-      </c>
-      <c r="L14" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B15" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D15" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B16" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" t="s">
         <v>49</v>
       </c>
-      <c r="F16" t="s">
+      <c r="J16" t="s">
         <v>50</v>
       </c>
-      <c r="G16" t="s">
+      <c r="K16" t="s">
         <v>51</v>
       </c>
-      <c r="H16" t="s">
-        <v>52</v>
-      </c>
-      <c r="I16" t="s">
-        <v>53</v>
-      </c>
-      <c r="J16" t="s">
-        <v>54</v>
-      </c>
-      <c r="K16" t="s">
-        <v>55</v>
-      </c>
-      <c r="L16" t="s">
-        <v>222</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>223</v>
-      </c>
+      <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
@@ -1791,75 +1799,75 @@
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="B17" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C17" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" t="s">
+        <v>26</v>
+      </c>
+      <c r="L17" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" t="s">
+        <v>28</v>
+      </c>
+      <c r="N17" t="s">
+        <v>17</v>
+      </c>
+      <c r="O17" t="s">
+        <v>18</v>
+      </c>
+      <c r="P17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q17" t="s">
         <v>20</v>
       </c>
-      <c r="F17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I17" t="s">
-        <v>28</v>
-      </c>
-      <c r="J17" t="s">
-        <v>29</v>
-      </c>
-      <c r="K17" t="s">
-        <v>30</v>
-      </c>
-      <c r="L17" t="s">
-        <v>31</v>
-      </c>
-      <c r="M17" t="s">
-        <v>32</v>
-      </c>
-      <c r="N17" t="s">
-        <v>21</v>
-      </c>
-      <c r="O17" t="s">
-        <v>22</v>
-      </c>
-      <c r="P17" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>24</v>
-      </c>
       <c r="R17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="S17" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="T17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B18" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -1877,7 +1885,7 @@
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
@@ -1897,16 +1905,16 @@
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B19" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C19" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -1924,7 +1932,7 @@
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
       <c r="U19" s="3" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
@@ -1944,16 +1952,16 @@
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B20" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1971,7 +1979,7 @@
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
       <c r="U20" s="3" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
@@ -1991,16 +1999,16 @@
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B21" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="C21" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -2018,7 +2026,7 @@
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
       <c r="U21" s="3" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
@@ -2038,238 +2046,258 @@
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B22" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="E22" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" t="s">
+        <v>68</v>
+      </c>
+      <c r="I22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J22" t="s">
+        <v>63</v>
+      </c>
+      <c r="K22" t="s">
+        <v>64</v>
+      </c>
+      <c r="L22" t="s">
         <v>69</v>
       </c>
-      <c r="F22" t="s">
+      <c r="M22" t="s">
         <v>70</v>
       </c>
-      <c r="G22" t="s">
+      <c r="N22" t="s">
         <v>71</v>
       </c>
-      <c r="H22" t="s">
+      <c r="O22" t="s">
         <v>72</v>
       </c>
-      <c r="I22" t="s">
-        <v>66</v>
-      </c>
-      <c r="J22" t="s">
-        <v>67</v>
-      </c>
-      <c r="K22" t="s">
-        <v>68</v>
-      </c>
-      <c r="L22" t="s">
+      <c r="P22" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>77</v>
+      </c>
+      <c r="R22" t="s">
+        <v>78</v>
+      </c>
+      <c r="S22" t="s">
+        <v>79</v>
+      </c>
+      <c r="T22" t="s">
         <v>73</v>
       </c>
-      <c r="M22" t="s">
+      <c r="U22" t="s">
         <v>74</v>
       </c>
-      <c r="N22" t="s">
+      <c r="V22" t="s">
         <v>75</v>
       </c>
-      <c r="O22" t="s">
-        <v>76</v>
-      </c>
-      <c r="P22" t="s">
+      <c r="W22" t="s">
         <v>80</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="X22" t="s">
         <v>81</v>
       </c>
-      <c r="R22" t="s">
+      <c r="Y22" t="s">
         <v>82</v>
       </c>
-      <c r="S22" t="s">
+      <c r="Z22" t="s">
         <v>83</v>
-      </c>
-      <c r="T22" t="s">
-        <v>77</v>
-      </c>
-      <c r="U22" t="s">
-        <v>78</v>
-      </c>
-      <c r="V22" t="s">
-        <v>79</v>
-      </c>
-      <c r="W22" t="s">
-        <v>84</v>
-      </c>
-      <c r="X22" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>175</v>
+        <v>168</v>
+      </c>
+      <c r="B23" t="s">
+        <v>229</v>
+      </c>
+      <c r="E23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" t="s">
+        <v>129</v>
+      </c>
+      <c r="G23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" t="s">
+        <v>52</v>
+      </c>
+      <c r="I23" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B24" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B25" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B26" t="s">
+        <v>196</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B27" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B28" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="B29" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="E29" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>231</v>
+      </c>
+      <c r="B30" t="s">
+        <v>230</v>
+      </c>
+      <c r="E30" t="s">
+        <v>228</v>
+      </c>
+      <c r="F30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" t="s">
+        <v>84</v>
+      </c>
       <c r="I30" t="s">
-        <v>57</v>
+        <v>13</v>
+      </c>
+      <c r="J30" t="s">
+        <v>14</v>
+      </c>
+      <c r="K30" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>232</v>
+      </c>
       <c r="B31" t="s">
-        <v>197</v>
-      </c>
-      <c r="I31" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>198</v>
-      </c>
-      <c r="I32" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I33" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I34" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I35" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I36" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I37" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I38" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I39" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I40" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I41" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I42" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="43" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I43" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I44" t="s">
-        <v>19</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="C31" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" t="s">
+        <v>234</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AA31" s="3"/>
+      <c r="AB31" s="3"/>
+      <c r="AC31" s="3"/>
+      <c r="AD31" s="3"/>
+      <c r="AE31" s="3"/>
+      <c r="AF31" s="3"/>
+      <c r="AG31" s="3"/>
+      <c r="AH31" s="3"/>
+      <c r="AI31" s="3"/>
+      <c r="AJ31" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="22">
+    <mergeCell ref="E31:AJ31"/>
+    <mergeCell ref="E3:L3"/>
+    <mergeCell ref="E8:T8"/>
+    <mergeCell ref="U8:AJ8"/>
+    <mergeCell ref="E9:T9"/>
+    <mergeCell ref="U9:AJ9"/>
     <mergeCell ref="E19:T19"/>
     <mergeCell ref="E20:T20"/>
     <mergeCell ref="E21:T21"/>
@@ -2282,13 +2310,10 @@
     <mergeCell ref="E2:L2"/>
     <mergeCell ref="M2:T2"/>
     <mergeCell ref="U2:AJ2"/>
-    <mergeCell ref="D3:L3"/>
     <mergeCell ref="M3:T3"/>
     <mergeCell ref="U3:AB3"/>
     <mergeCell ref="AC3:AJ3"/>
     <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E8:AJ8"/>
-    <mergeCell ref="E9:AJ9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
version 3.2,fixed ADC module and diagnostic UART ,tested
</commit_message>
<xml_diff>
--- a/HSID_RCB_RevB.xlsx
+++ b/HSID_RCB_RevB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\FPGA\git\RCB_Rev_B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4911CED9-EBDF-46FD-8C8E-0A1D48E53CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203F748D-5F1E-46B7-B0B8-66B989B647FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9B9F24D7-41B0-450D-BA52-4B08206AAC62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9B9F24D7-41B0-450D-BA52-4B08206AAC62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="239">
   <si>
     <t>reg</t>
   </si>
@@ -750,6 +750,9 @@
   </si>
   <si>
     <t>Right Diagnostic counter</t>
+  </si>
+  <si>
+    <t>TBD</t>
   </si>
 </sst>
 </file>
@@ -777,7 +780,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -787,6 +790,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -808,16 +817,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1154,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B1DA1C-2C46-416D-A8B7-01E6D657AEE6}">
   <dimension ref="A1:AJ31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,106 +1291,111 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="D2" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6" t="s">
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="6"/>
-      <c r="AG2" s="6"/>
-      <c r="AH2" s="6"/>
-      <c r="AI2" s="6"/>
-      <c r="AJ2" s="6"/>
-    </row>
-    <row r="3" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="7"/>
+      <c r="AH2" s="7"/>
+      <c r="AI2" s="7"/>
+      <c r="AJ2" s="7"/>
+    </row>
+    <row r="3" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6" t="s">
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6" t="s">
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="6"/>
-      <c r="AH3" s="6"/>
-      <c r="AI3" s="6"/>
-      <c r="AJ3" s="6"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="7"/>
+      <c r="AH3" s="7"/>
+      <c r="AI3" s="7"/>
+      <c r="AJ3" s="7"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1388,366 +1404,408 @@
       <c r="B4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="5" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="C4" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="D6" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="N6" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="P6" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="7" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="D7" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="O7" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="P7" s="5" t="s">
+      <c r="P7" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3" t="s">
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
-      <c r="AE8" s="3"/>
-      <c r="AF8" s="3"/>
-      <c r="AG8" s="3"/>
-      <c r="AH8" s="3"/>
-      <c r="AI8" s="3"/>
-      <c r="AJ8" s="3"/>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="7"/>
+    </row>
+    <row r="9" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3" t="s">
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-      <c r="AC9" s="3"/>
-      <c r="AD9" s="3"/>
-      <c r="AE9" s="3"/>
-      <c r="AF9" s="3"/>
-      <c r="AG9" s="3"/>
-      <c r="AH9" s="3"/>
-      <c r="AI9" s="3"/>
-      <c r="AJ9" s="3"/>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="7"/>
+      <c r="AH9" s="7"/>
+      <c r="AI9" s="7"/>
+      <c r="AJ9" s="7"/>
+    </row>
+    <row r="10" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="E10" t="s">
+      <c r="C10" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="E11" t="s">
+      <c r="C11" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="D12" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="D13" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E14" t="s">
+      <c r="D14" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1759,6 +1817,9 @@
       <c r="C16" t="s">
         <v>91</v>
       </c>
+      <c r="D16" s="2" t="s">
+        <v>238</v>
+      </c>
       <c r="E16" t="s">
         <v>45</v>
       </c>
@@ -1780,269 +1841,284 @@
       <c r="K16" t="s">
         <v>51</v>
       </c>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
-      <c r="X16" s="3"/>
-      <c r="Y16" s="3"/>
-      <c r="Z16" s="3"/>
-      <c r="AA16" s="3"/>
-      <c r="AB16" s="3"/>
-    </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="6"/>
+    </row>
+    <row r="17" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E17" t="s">
+      <c r="D17" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O17" t="s">
+      <c r="O17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="Q17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="R17" t="s">
+      <c r="R17" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="S17" t="s">
+      <c r="S17" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="T17" t="s">
+      <c r="T17" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="D18" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3" t="s">
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
-      <c r="Z18" s="3"/>
-      <c r="AA18" s="3"/>
-      <c r="AB18" s="3"/>
-      <c r="AC18" s="3"/>
-      <c r="AD18" s="3"/>
-      <c r="AE18" s="3"/>
-      <c r="AF18" s="3"/>
-      <c r="AG18" s="3"/>
-      <c r="AH18" s="3"/>
-      <c r="AI18" s="3"/>
-      <c r="AJ18" s="3"/>
-    </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
+      <c r="AB18" s="7"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="7"/>
+      <c r="AE18" s="7"/>
+      <c r="AF18" s="7"/>
+      <c r="AG18" s="7"/>
+      <c r="AH18" s="7"/>
+      <c r="AI18" s="7"/>
+      <c r="AJ18" s="7"/>
+    </row>
+    <row r="19" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="D19" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3" t="s">
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
-      <c r="Y19" s="3"/>
-      <c r="Z19" s="3"/>
-      <c r="AA19" s="3"/>
-      <c r="AB19" s="3"/>
-      <c r="AC19" s="3"/>
-      <c r="AD19" s="3"/>
-      <c r="AE19" s="3"/>
-      <c r="AF19" s="3"/>
-      <c r="AG19" s="3"/>
-      <c r="AH19" s="3"/>
-      <c r="AI19" s="3"/>
-      <c r="AJ19" s="3"/>
-    </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="7"/>
+      <c r="AC19" s="7"/>
+      <c r="AD19" s="7"/>
+      <c r="AE19" s="7"/>
+      <c r="AF19" s="7"/>
+      <c r="AG19" s="7"/>
+      <c r="AH19" s="7"/>
+      <c r="AI19" s="7"/>
+      <c r="AJ19" s="7"/>
+    </row>
+    <row r="20" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="D20" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3" t="s">
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
-      <c r="AA20" s="3"/>
-      <c r="AB20" s="3"/>
-      <c r="AC20" s="3"/>
-      <c r="AD20" s="3"/>
-      <c r="AE20" s="3"/>
-      <c r="AF20" s="3"/>
-      <c r="AG20" s="3"/>
-      <c r="AH20" s="3"/>
-      <c r="AI20" s="3"/>
-      <c r="AJ20" s="3"/>
-    </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="7"/>
+      <c r="AC20" s="7"/>
+      <c r="AD20" s="7"/>
+      <c r="AE20" s="7"/>
+      <c r="AF20" s="7"/>
+      <c r="AG20" s="7"/>
+      <c r="AH20" s="7"/>
+      <c r="AI20" s="7"/>
+      <c r="AJ20" s="7"/>
+    </row>
+    <row r="21" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="D21" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3" t="s">
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="V21" s="3"/>
-      <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
-      <c r="Z21" s="3"/>
-      <c r="AA21" s="3"/>
-      <c r="AB21" s="3"/>
-      <c r="AC21" s="3"/>
-      <c r="AD21" s="3"/>
-      <c r="AE21" s="3"/>
-      <c r="AF21" s="3"/>
-      <c r="AG21" s="3"/>
-      <c r="AH21" s="3"/>
-      <c r="AI21" s="3"/>
-      <c r="AJ21" s="3"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="7"/>
+      <c r="AA21" s="7"/>
+      <c r="AB21" s="7"/>
+      <c r="AC21" s="7"/>
+      <c r="AD21" s="7"/>
+      <c r="AE21" s="7"/>
+      <c r="AF21" s="7"/>
+      <c r="AG21" s="7"/>
+      <c r="AH21" s="7"/>
+      <c r="AI21" s="7"/>
+      <c r="AJ21" s="7"/>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2051,6 +2127,12 @@
       <c r="B22" t="s">
         <v>225</v>
       </c>
+      <c r="C22" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>238</v>
+      </c>
       <c r="E22" t="s">
         <v>65</v>
       </c>
@@ -2125,6 +2207,12 @@
       <c r="B23" t="s">
         <v>229</v>
       </c>
+      <c r="C23" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>238</v>
+      </c>
       <c r="E23" t="s">
         <v>15</v>
       </c>
@@ -2141,53 +2229,77 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="C24" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="C25" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="C26" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="C27" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>204</v>
       </c>
     </row>
@@ -2198,6 +2310,12 @@
       <c r="B28" t="s">
         <v>198</v>
       </c>
+      <c r="C28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>238</v>
+      </c>
       <c r="E28" s="1" t="s">
         <v>203</v>
       </c>
@@ -2209,6 +2327,12 @@
       <c r="B29" t="s">
         <v>199</v>
       </c>
+      <c r="C29" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>238</v>
+      </c>
       <c r="E29" t="s">
         <v>202</v>
       </c>
@@ -2220,6 +2344,12 @@
       <c r="B30" t="s">
         <v>230</v>
       </c>
+      <c r="C30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>238</v>
+      </c>
       <c r="E30" t="s">
         <v>228</v>
       </c>
@@ -2255,43 +2385,49 @@
       <c r="D31" t="s">
         <v>234</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="3"/>
-      <c r="S31" s="3"/>
-      <c r="T31" s="3"/>
-      <c r="U31" s="3"/>
-      <c r="V31" s="3"/>
-      <c r="W31" s="3"/>
-      <c r="X31" s="3"/>
-      <c r="Y31" s="3"/>
-      <c r="Z31" s="3"/>
-      <c r="AA31" s="3"/>
-      <c r="AB31" s="3"/>
-      <c r="AC31" s="3"/>
-      <c r="AD31" s="3"/>
-      <c r="AE31" s="3"/>
-      <c r="AF31" s="3"/>
-      <c r="AG31" s="3"/>
-      <c r="AH31" s="3"/>
-      <c r="AI31" s="3"/>
-      <c r="AJ31" s="3"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="6"/>
+      <c r="U31" s="6"/>
+      <c r="V31" s="6"/>
+      <c r="W31" s="6"/>
+      <c r="X31" s="6"/>
+      <c r="Y31" s="6"/>
+      <c r="Z31" s="6"/>
+      <c r="AA31" s="6"/>
+      <c r="AB31" s="6"/>
+      <c r="AC31" s="6"/>
+      <c r="AD31" s="6"/>
+      <c r="AE31" s="6"/>
+      <c r="AF31" s="6"/>
+      <c r="AG31" s="6"/>
+      <c r="AH31" s="6"/>
+      <c r="AI31" s="6"/>
+      <c r="AJ31" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="E2:L2"/>
+    <mergeCell ref="M2:T2"/>
+    <mergeCell ref="U2:AJ2"/>
+    <mergeCell ref="M3:T3"/>
+    <mergeCell ref="U3:AB3"/>
+    <mergeCell ref="AC3:AJ3"/>
     <mergeCell ref="E31:AJ31"/>
     <mergeCell ref="E3:L3"/>
     <mergeCell ref="E8:T8"/>
@@ -2307,12 +2443,6 @@
     <mergeCell ref="M16:AB16"/>
     <mergeCell ref="E18:T18"/>
     <mergeCell ref="U18:AJ18"/>
-    <mergeCell ref="E2:L2"/>
-    <mergeCell ref="M2:T2"/>
-    <mergeCell ref="U2:AJ2"/>
-    <mergeCell ref="M3:T3"/>
-    <mergeCell ref="U3:AB3"/>
-    <mergeCell ref="AC3:AJ3"/>
     <mergeCell ref="E15:G15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
fixed and tested diagnostic ,new ADC I2c module implemented TODO:fix i2c read,verify FPGA pinout
</commit_message>
<xml_diff>
--- a/HSID_RCB_RevB.xlsx
+++ b/HSID_RCB_RevB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\FPGA\git\RCB_Rev_B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203F748D-5F1E-46B7-B0B8-66B989B647FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731007AC-1251-46BA-8F25-72AD7AD12556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9B9F24D7-41B0-450D-BA52-4B08206AAC62}"/>
+    <workbookView minimized="1" xWindow="30" yWindow="0" windowWidth="28770" windowHeight="15300" xr2:uid="{9B9F24D7-41B0-450D-BA52-4B08206AAC62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -800,7 +800,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -808,11 +808,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -823,10 +838,13 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1165,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B1DA1C-2C46-416D-A8B7-01E6D657AEE6}">
   <dimension ref="A1:AJ31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,16 +1200,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>171</v>
       </c>
       <c r="E1" t="s">
@@ -1292,136 +1310,136 @@
       </c>
     </row>
     <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7" t="s">
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7" t="s">
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="7"/>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="7"/>
-      <c r="AH2" s="7"/>
-      <c r="AI2" s="7"/>
-      <c r="AJ2" s="7"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="9"/>
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="9"/>
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="9"/>
     </row>
     <row r="3" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7" t="s">
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7" t="s">
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="7" t="s">
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="AD3" s="7"/>
-      <c r="AE3" s="7"/>
-      <c r="AF3" s="7"/>
-      <c r="AG3" s="7"/>
-      <c r="AH3" s="7"/>
-      <c r="AI3" s="7"/>
-      <c r="AJ3" s="7"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="9"/>
+      <c r="AG3" s="9"/>
+      <c r="AH3" s="9"/>
+      <c r="AI3" s="9"/>
+      <c r="AJ3" s="9"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="7" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="7" t="s">
         <v>238</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -1438,16 +1456,16 @@
       </c>
     </row>
     <row r="6" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="7" t="s">
         <v>238</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -1488,16 +1506,16 @@
       </c>
     </row>
     <row r="7" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="7" t="s">
         <v>238</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -1538,116 +1556,116 @@
       </c>
     </row>
     <row r="8" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E8" s="7" t="s">
+      <c r="D8" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7" t="s">
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
-      <c r="Y8" s="7"/>
-      <c r="Z8" s="7"/>
-      <c r="AA8" s="7"/>
-      <c r="AB8" s="7"/>
-      <c r="AC8" s="7"/>
-      <c r="AD8" s="7"/>
-      <c r="AE8" s="7"/>
-      <c r="AF8" s="7"/>
-      <c r="AG8" s="7"/>
-      <c r="AH8" s="7"/>
-      <c r="AI8" s="7"/>
-      <c r="AJ8" s="7"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="9"/>
+      <c r="AG8" s="9"/>
+      <c r="AH8" s="9"/>
+      <c r="AI8" s="9"/>
+      <c r="AJ8" s="9"/>
     </row>
     <row r="9" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E9" s="7" t="s">
+      <c r="D9" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7" t="s">
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="7"/>
-      <c r="Z9" s="7"/>
-      <c r="AA9" s="7"/>
-      <c r="AB9" s="7"/>
-      <c r="AC9" s="7"/>
-      <c r="AD9" s="7"/>
-      <c r="AE9" s="7"/>
-      <c r="AF9" s="7"/>
-      <c r="AG9" s="7"/>
-      <c r="AH9" s="7"/>
-      <c r="AI9" s="7"/>
-      <c r="AJ9" s="7"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9"/>
+      <c r="AI9" s="9"/>
+      <c r="AJ9" s="9"/>
     </row>
     <row r="10" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="7" t="s">
         <v>238</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -1667,16 +1685,16 @@
       </c>
     </row>
     <row r="11" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="7" t="s">
         <v>238</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -1696,16 +1714,16 @@
       </c>
     </row>
     <row r="12" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="7" t="s">
         <v>238</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -1722,16 +1740,16 @@
       </c>
     </row>
     <row r="13" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="7" t="s">
         <v>238</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -1751,16 +1769,16 @@
       </c>
     </row>
     <row r="14" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="7" t="s">
         <v>238</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -1789,35 +1807,35 @@
       </c>
     </row>
     <row r="15" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="7" t="s">
         <v>238</v>
       </c>
       <c r="E16" t="s">
@@ -1841,34 +1859,34 @@
       <c r="K16" t="s">
         <v>51</v>
       </c>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
-      <c r="U16" s="6"/>
-      <c r="V16" s="6"/>
-      <c r="W16" s="6"/>
-      <c r="X16" s="6"/>
-      <c r="Y16" s="6"/>
-      <c r="Z16" s="6"/>
-      <c r="AA16" s="6"/>
-      <c r="AB16" s="6"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="10"/>
+      <c r="AB16" s="10"/>
     </row>
     <row r="17" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="7" t="s">
         <v>238</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -1921,216 +1939,216 @@
       </c>
     </row>
     <row r="18" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E18" s="7" t="s">
+      <c r="D18" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E18" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
-      <c r="U18" s="7" t="s">
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
-      <c r="X18" s="7"/>
-      <c r="Y18" s="7"/>
-      <c r="Z18" s="7"/>
-      <c r="AA18" s="7"/>
-      <c r="AB18" s="7"/>
-      <c r="AC18" s="7"/>
-      <c r="AD18" s="7"/>
-      <c r="AE18" s="7"/>
-      <c r="AF18" s="7"/>
-      <c r="AG18" s="7"/>
-      <c r="AH18" s="7"/>
-      <c r="AI18" s="7"/>
-      <c r="AJ18" s="7"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
+      <c r="AA18" s="9"/>
+      <c r="AB18" s="9"/>
+      <c r="AC18" s="9"/>
+      <c r="AD18" s="9"/>
+      <c r="AE18" s="9"/>
+      <c r="AF18" s="9"/>
+      <c r="AG18" s="9"/>
+      <c r="AH18" s="9"/>
+      <c r="AI18" s="9"/>
+      <c r="AJ18" s="9"/>
     </row>
     <row r="19" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E19" s="7" t="s">
+      <c r="D19" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="7" t="s">
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="V19" s="7"/>
-      <c r="W19" s="7"/>
-      <c r="X19" s="7"/>
-      <c r="Y19" s="7"/>
-      <c r="Z19" s="7"/>
-      <c r="AA19" s="7"/>
-      <c r="AB19" s="7"/>
-      <c r="AC19" s="7"/>
-      <c r="AD19" s="7"/>
-      <c r="AE19" s="7"/>
-      <c r="AF19" s="7"/>
-      <c r="AG19" s="7"/>
-      <c r="AH19" s="7"/>
-      <c r="AI19" s="7"/>
-      <c r="AJ19" s="7"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
+      <c r="AB19" s="9"/>
+      <c r="AC19" s="9"/>
+      <c r="AD19" s="9"/>
+      <c r="AE19" s="9"/>
+      <c r="AF19" s="9"/>
+      <c r="AG19" s="9"/>
+      <c r="AH19" s="9"/>
+      <c r="AI19" s="9"/>
+      <c r="AJ19" s="9"/>
     </row>
     <row r="20" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E20" s="7" t="s">
+      <c r="D20" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="7" t="s">
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="V20" s="7"/>
-      <c r="W20" s="7"/>
-      <c r="X20" s="7"/>
-      <c r="Y20" s="7"/>
-      <c r="Z20" s="7"/>
-      <c r="AA20" s="7"/>
-      <c r="AB20" s="7"/>
-      <c r="AC20" s="7"/>
-      <c r="AD20" s="7"/>
-      <c r="AE20" s="7"/>
-      <c r="AF20" s="7"/>
-      <c r="AG20" s="7"/>
-      <c r="AH20" s="7"/>
-      <c r="AI20" s="7"/>
-      <c r="AJ20" s="7"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
+      <c r="AB20" s="9"/>
+      <c r="AC20" s="9"/>
+      <c r="AD20" s="9"/>
+      <c r="AE20" s="9"/>
+      <c r="AF20" s="9"/>
+      <c r="AG20" s="9"/>
+      <c r="AH20" s="9"/>
+      <c r="AI20" s="9"/>
+      <c r="AJ20" s="9"/>
     </row>
     <row r="21" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E21" s="7" t="s">
+      <c r="D21" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="7" t="s">
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="V21" s="7"/>
-      <c r="W21" s="7"/>
-      <c r="X21" s="7"/>
-      <c r="Y21" s="7"/>
-      <c r="Z21" s="7"/>
-      <c r="AA21" s="7"/>
-      <c r="AB21" s="7"/>
-      <c r="AC21" s="7"/>
-      <c r="AD21" s="7"/>
-      <c r="AE21" s="7"/>
-      <c r="AF21" s="7"/>
-      <c r="AG21" s="7"/>
-      <c r="AH21" s="7"/>
-      <c r="AI21" s="7"/>
-      <c r="AJ21" s="7"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+      <c r="AB21" s="9"/>
+      <c r="AC21" s="9"/>
+      <c r="AD21" s="9"/>
+      <c r="AE21" s="9"/>
+      <c r="AF21" s="9"/>
+      <c r="AG21" s="9"/>
+      <c r="AH21" s="9"/>
+      <c r="AI21" s="9"/>
+      <c r="AJ21" s="9"/>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="7" t="s">
         <v>238</v>
       </c>
       <c r="E22" t="s">
@@ -2201,16 +2219,16 @@
       </c>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="7" t="s">
         <v>238</v>
       </c>
       <c r="E23" t="s">
@@ -2230,16 +2248,16 @@
       </c>
     </row>
     <row r="24" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="7" t="s">
         <v>238</v>
       </c>
       <c r="E24" s="3" t="s">
@@ -2250,16 +2268,16 @@
       </c>
     </row>
     <row r="25" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="7" t="s">
         <v>238</v>
       </c>
       <c r="E25" s="4" t="s">
@@ -2267,16 +2285,16 @@
       </c>
     </row>
     <row r="26" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="7" t="s">
         <v>238</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -2287,16 +2305,16 @@
       </c>
     </row>
     <row r="27" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="7" t="s">
         <v>238</v>
       </c>
       <c r="E27" s="4" t="s">
@@ -2304,16 +2322,16 @@
       </c>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="7" t="s">
         <v>238</v>
       </c>
       <c r="E28" s="1" t="s">
@@ -2321,16 +2339,16 @@
       </c>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="7" t="s">
         <v>238</v>
       </c>
       <c r="E29" t="s">
@@ -2338,16 +2356,16 @@
       </c>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="7" t="s">
         <v>238</v>
       </c>
       <c r="E30" t="s">
@@ -2373,61 +2391,55 @@
       </c>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
-      <c r="Q31" s="6"/>
-      <c r="R31" s="6"/>
-      <c r="S31" s="6"/>
-      <c r="T31" s="6"/>
-      <c r="U31" s="6"/>
-      <c r="V31" s="6"/>
-      <c r="W31" s="6"/>
-      <c r="X31" s="6"/>
-      <c r="Y31" s="6"/>
-      <c r="Z31" s="6"/>
-      <c r="AA31" s="6"/>
-      <c r="AB31" s="6"/>
-      <c r="AC31" s="6"/>
-      <c r="AD31" s="6"/>
-      <c r="AE31" s="6"/>
-      <c r="AF31" s="6"/>
-      <c r="AG31" s="6"/>
-      <c r="AH31" s="6"/>
-      <c r="AI31" s="6"/>
-      <c r="AJ31" s="6"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="10"/>
+      <c r="V31" s="10"/>
+      <c r="W31" s="10"/>
+      <c r="X31" s="10"/>
+      <c r="Y31" s="10"/>
+      <c r="Z31" s="10"/>
+      <c r="AA31" s="10"/>
+      <c r="AB31" s="10"/>
+      <c r="AC31" s="10"/>
+      <c r="AD31" s="10"/>
+      <c r="AE31" s="10"/>
+      <c r="AF31" s="10"/>
+      <c r="AG31" s="10"/>
+      <c r="AH31" s="10"/>
+      <c r="AI31" s="10"/>
+      <c r="AJ31" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="E2:L2"/>
-    <mergeCell ref="M2:T2"/>
-    <mergeCell ref="U2:AJ2"/>
-    <mergeCell ref="M3:T3"/>
-    <mergeCell ref="U3:AB3"/>
-    <mergeCell ref="AC3:AJ3"/>
     <mergeCell ref="E31:AJ31"/>
     <mergeCell ref="E3:L3"/>
     <mergeCell ref="E8:T8"/>
@@ -2444,6 +2456,12 @@
     <mergeCell ref="E18:T18"/>
     <mergeCell ref="U18:AJ18"/>
     <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E2:L2"/>
+    <mergeCell ref="M2:T2"/>
+    <mergeCell ref="U2:AJ2"/>
+    <mergeCell ref="M3:T3"/>
+    <mergeCell ref="U3:AB3"/>
+    <mergeCell ref="AC3:AJ3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added header register,see more info in HSID_RCB_RevB ,version 0x0307
</commit_message>
<xml_diff>
--- a/HSID_RCB_RevB.xlsx
+++ b/HSID_RCB_RevB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\FPGA\git\RCB_Rev_B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731007AC-1251-46BA-8F25-72AD7AD12556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A062C8E4-1ED2-4CF8-A5DA-1CB7E9E4CF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="30" yWindow="0" windowWidth="28770" windowHeight="15300" xr2:uid="{9B9F24D7-41B0-450D-BA52-4B08206AAC62}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9B9F24D7-41B0-450D-BA52-4B08206AAC62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="243">
   <si>
     <t>reg</t>
   </si>
@@ -753,6 +753,18 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>spare</t>
+  </si>
+  <si>
+    <t>Diagnostic_Header</t>
+  </si>
+  <si>
+    <t>0x001E</t>
+  </si>
+  <si>
+    <t>Diagnostic Header IOs,Input:FPGA1-4+Teensy_FPGA_SP0-2 ,output: FPGA5-13</t>
   </si>
 </sst>
 </file>
@@ -800,7 +812,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -823,11 +835,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -847,6 +870,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1181,10 +1205,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B1DA1C-2C46-416D-A8B7-01E6D657AEE6}">
-  <dimension ref="A1:AJ31"/>
+  <dimension ref="A1:AJ32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,6 +1477,18 @@
       </c>
       <c r="H5" s="2" t="s">
         <v>57</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2438,6 +2474,68 @@
       <c r="AI31" s="10"/>
       <c r="AJ31" s="10"/>
     </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I32" t="s">
+        <v>85</v>
+      </c>
+      <c r="J32" t="s">
+        <v>86</v>
+      </c>
+      <c r="K32" t="s">
+        <v>87</v>
+      </c>
+      <c r="L32" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M32" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="N32" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="O32" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P32" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q32" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="R32" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="S32" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="T32" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="22">
     <mergeCell ref="E31:AJ31"/>
@@ -2465,5 +2563,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added FPGA control register,version:0409
</commit_message>
<xml_diff>
--- a/HSID_RCB_RevB.xlsx
+++ b/HSID_RCB_RevB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\FPGA\git\RCB_Rev_B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A062C8E4-1ED2-4CF8-A5DA-1CB7E9E4CF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76C5D05-08D4-41C8-8E90-1449A7A55F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9B9F24D7-41B0-450D-BA52-4B08206AAC62}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="246">
   <si>
     <t>reg</t>
   </si>
@@ -765,6 +765,15 @@
   </si>
   <si>
     <t>Diagnostic Header IOs,Input:FPGA1-4+Teensy_FPGA_SP0-2 ,output: FPGA5-13</t>
+  </si>
+  <si>
+    <t>0x001F</t>
+  </si>
+  <si>
+    <t>FPGA Control register</t>
+  </si>
+  <si>
+    <t>Diagnostic UART Reset(active high)</t>
   </si>
 </sst>
 </file>
@@ -812,7 +821,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -846,11 +855,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -864,13 +882,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1205,10 +1224,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B1DA1C-2C46-416D-A8B7-01E6D657AEE6}">
-  <dimension ref="A1:AJ32"/>
+  <dimension ref="A1:AJ33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,44 +1365,44 @@
       <c r="D2" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9" t="s">
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9" t="s">
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="9"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="11"/>
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="11"/>
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="11"/>
+      <c r="AG2" s="11"/>
+      <c r="AH2" s="11"/>
+      <c r="AI2" s="11"/>
+      <c r="AJ2" s="11"/>
     </row>
     <row r="3" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -1398,46 +1417,46 @@
       <c r="D3" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9" t="s">
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9" t="s">
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="AD3" s="9"/>
-      <c r="AE3" s="9"/>
-      <c r="AF3" s="9"/>
-      <c r="AG3" s="9"/>
-      <c r="AH3" s="9"/>
-      <c r="AI3" s="9"/>
-      <c r="AJ3" s="9"/>
+      <c r="AD3" s="11"/>
+      <c r="AE3" s="11"/>
+      <c r="AF3" s="11"/>
+      <c r="AG3" s="11"/>
+      <c r="AH3" s="11"/>
+      <c r="AI3" s="11"/>
+      <c r="AJ3" s="11"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -1604,42 +1623,42 @@
       <c r="D8" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9" t="s">
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9"/>
-      <c r="Y8" s="9"/>
-      <c r="Z8" s="9"/>
-      <c r="AA8" s="9"/>
-      <c r="AB8" s="9"/>
-      <c r="AC8" s="9"/>
-      <c r="AD8" s="9"/>
-      <c r="AE8" s="9"/>
-      <c r="AF8" s="9"/>
-      <c r="AG8" s="9"/>
-      <c r="AH8" s="9"/>
-      <c r="AI8" s="9"/>
-      <c r="AJ8" s="9"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="11"/>
+      <c r="AD8" s="11"/>
+      <c r="AE8" s="11"/>
+      <c r="AF8" s="11"/>
+      <c r="AG8" s="11"/>
+      <c r="AH8" s="11"/>
+      <c r="AI8" s="11"/>
+      <c r="AJ8" s="11"/>
     </row>
     <row r="9" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -1654,42 +1673,42 @@
       <c r="D9" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9" t="s">
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="V9" s="9"/>
-      <c r="W9" s="9"/>
-      <c r="X9" s="9"/>
-      <c r="Y9" s="9"/>
-      <c r="Z9" s="9"/>
-      <c r="AA9" s="9"/>
-      <c r="AB9" s="9"/>
-      <c r="AC9" s="9"/>
-      <c r="AD9" s="9"/>
-      <c r="AE9" s="9"/>
-      <c r="AF9" s="9"/>
-      <c r="AG9" s="9"/>
-      <c r="AH9" s="9"/>
-      <c r="AI9" s="9"/>
-      <c r="AJ9" s="9"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="11"/>
+      <c r="AC9" s="11"/>
+      <c r="AD9" s="11"/>
+      <c r="AE9" s="11"/>
+      <c r="AF9" s="11"/>
+      <c r="AG9" s="11"/>
+      <c r="AH9" s="11"/>
+      <c r="AI9" s="11"/>
+      <c r="AJ9" s="11"/>
     </row>
     <row r="10" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -1855,11 +1874,11 @@
       <c r="D15" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
@@ -1987,42 +2006,42 @@
       <c r="D18" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
-      <c r="U18" s="9" t="s">
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="V18" s="9"/>
-      <c r="W18" s="9"/>
-      <c r="X18" s="9"/>
-      <c r="Y18" s="9"/>
-      <c r="Z18" s="9"/>
-      <c r="AA18" s="9"/>
-      <c r="AB18" s="9"/>
-      <c r="AC18" s="9"/>
-      <c r="AD18" s="9"/>
-      <c r="AE18" s="9"/>
-      <c r="AF18" s="9"/>
-      <c r="AG18" s="9"/>
-      <c r="AH18" s="9"/>
-      <c r="AI18" s="9"/>
-      <c r="AJ18" s="9"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="11"/>
+      <c r="AE18" s="11"/>
+      <c r="AF18" s="11"/>
+      <c r="AG18" s="11"/>
+      <c r="AH18" s="11"/>
+      <c r="AI18" s="11"/>
+      <c r="AJ18" s="11"/>
     </row>
     <row r="19" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
@@ -2037,42 +2056,42 @@
       <c r="D19" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="9" t="s">
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
-      <c r="X19" s="9"/>
-      <c r="Y19" s="9"/>
-      <c r="Z19" s="9"/>
-      <c r="AA19" s="9"/>
-      <c r="AB19" s="9"/>
-      <c r="AC19" s="9"/>
-      <c r="AD19" s="9"/>
-      <c r="AE19" s="9"/>
-      <c r="AF19" s="9"/>
-      <c r="AG19" s="9"/>
-      <c r="AH19" s="9"/>
-      <c r="AI19" s="9"/>
-      <c r="AJ19" s="9"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="11"/>
+      <c r="AC19" s="11"/>
+      <c r="AD19" s="11"/>
+      <c r="AE19" s="11"/>
+      <c r="AF19" s="11"/>
+      <c r="AG19" s="11"/>
+      <c r="AH19" s="11"/>
+      <c r="AI19" s="11"/>
+      <c r="AJ19" s="11"/>
     </row>
     <row r="20" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
@@ -2087,42 +2106,42 @@
       <c r="D20" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9" t="s">
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
-      <c r="X20" s="9"/>
-      <c r="Y20" s="9"/>
-      <c r="Z20" s="9"/>
-      <c r="AA20" s="9"/>
-      <c r="AB20" s="9"/>
-      <c r="AC20" s="9"/>
-      <c r="AD20" s="9"/>
-      <c r="AE20" s="9"/>
-      <c r="AF20" s="9"/>
-      <c r="AG20" s="9"/>
-      <c r="AH20" s="9"/>
-      <c r="AI20" s="9"/>
-      <c r="AJ20" s="9"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="11"/>
+      <c r="AB20" s="11"/>
+      <c r="AC20" s="11"/>
+      <c r="AD20" s="11"/>
+      <c r="AE20" s="11"/>
+      <c r="AF20" s="11"/>
+      <c r="AG20" s="11"/>
+      <c r="AH20" s="11"/>
+      <c r="AI20" s="11"/>
+      <c r="AJ20" s="11"/>
     </row>
     <row r="21" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
@@ -2137,42 +2156,42 @@
       <c r="D21" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
-      <c r="U21" s="9" t="s">
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
-      <c r="X21" s="9"/>
-      <c r="Y21" s="9"/>
-      <c r="Z21" s="9"/>
-      <c r="AA21" s="9"/>
-      <c r="AB21" s="9"/>
-      <c r="AC21" s="9"/>
-      <c r="AD21" s="9"/>
-      <c r="AE21" s="9"/>
-      <c r="AF21" s="9"/>
-      <c r="AG21" s="9"/>
-      <c r="AH21" s="9"/>
-      <c r="AI21" s="9"/>
-      <c r="AJ21" s="9"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+      <c r="X21" s="11"/>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="11"/>
+      <c r="AA21" s="11"/>
+      <c r="AB21" s="11"/>
+      <c r="AC21" s="11"/>
+      <c r="AD21" s="11"/>
+      <c r="AE21" s="11"/>
+      <c r="AF21" s="11"/>
+      <c r="AG21" s="11"/>
+      <c r="AH21" s="11"/>
+      <c r="AI21" s="11"/>
+      <c r="AJ21" s="11"/>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
@@ -2487,16 +2506,16 @@
       <c r="D32" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G32" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H32" s="11" t="s">
+      <c r="H32" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I32" t="s">
@@ -2508,36 +2527,59 @@
       <c r="K32" t="s">
         <v>87</v>
       </c>
-      <c r="L32" s="11" t="s">
+      <c r="L32" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="M32" s="11" t="s">
+      <c r="M32" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="N32" s="11" t="s">
+      <c r="N32" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="O32" s="11" t="s">
+      <c r="O32" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="P32" s="11" t="s">
+      <c r="P32" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="Q32" s="11" t="s">
+      <c r="Q32" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="R32" s="11" t="s">
+      <c r="R32" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="S32" s="11" t="s">
+      <c r="S32" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="T32" s="11" t="s">
+      <c r="T32" s="9" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="E2:L2"/>
+    <mergeCell ref="M2:T2"/>
+    <mergeCell ref="U2:AJ2"/>
+    <mergeCell ref="M3:T3"/>
+    <mergeCell ref="U3:AB3"/>
+    <mergeCell ref="AC3:AJ3"/>
     <mergeCell ref="E31:AJ31"/>
     <mergeCell ref="E3:L3"/>
     <mergeCell ref="E8:T8"/>
@@ -2554,12 +2596,6 @@
     <mergeCell ref="E18:T18"/>
     <mergeCell ref="U18:AJ18"/>
     <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E2:L2"/>
-    <mergeCell ref="M2:T2"/>
-    <mergeCell ref="U2:AJ2"/>
-    <mergeCell ref="M3:T3"/>
-    <mergeCell ref="U3:AB3"/>
-    <mergeCell ref="AC3:AJ3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>